<commit_message>
demo seed for three shops
Former-commit-id: 3dfc417dcca645db54876ab50e3634202c66891e
</commit_message>
<xml_diff>
--- a/db/dummydata/new_public_ocean_ptp_rates.xlsx
+++ b/db/dummydata/new_public_ocean_ptp_rates.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
   <si>
     <t>"BAS" =&gt; "Basic Ocean Freight",
       "HAS" =&gt; "HEAVY Ocean Freight",
@@ -81,90 +81,6 @@
     <t>LCL_HEAVY_WEIGHT_SURCHARGE_MIN</t>
   </si>
   <si>
-    <t>OHC_CURRENCY</t>
-  </si>
-  <si>
-    <t>OHC_CBM</t>
-  </si>
-  <si>
-    <t>OHC_TON</t>
-  </si>
-  <si>
-    <t>OHC_MIN</t>
-  </si>
-  <si>
-    <t>LCLS_CURRENCY</t>
-  </si>
-  <si>
-    <t>LCL_SERVICE_CBM</t>
-  </si>
-  <si>
-    <t>LCL_SERVICE_TON</t>
-  </si>
-  <si>
-    <t>LCL_SERVICE_MIN</t>
-  </si>
-  <si>
-    <t>ISPS_CURRENCY</t>
-  </si>
-  <si>
-    <t>ISPS</t>
-  </si>
-  <si>
-    <t>ODF_CURRENCY</t>
-  </si>
-  <si>
-    <t>ODF</t>
-  </si>
-  <si>
-    <t>LS_CURRENCY</t>
-  </si>
-  <si>
-    <t>LINER_SERVICE_FEE</t>
-  </si>
-  <si>
-    <t>VGM_CURRENCY</t>
-  </si>
-  <si>
-    <t>VGM_FEE</t>
-  </si>
-  <si>
-    <t>DDF_CURRENCY</t>
-  </si>
-  <si>
-    <t>DDF</t>
-  </si>
-  <si>
-    <t>DHC_CURRENCY</t>
-  </si>
-  <si>
-    <t>DHC</t>
-  </si>
-  <si>
-    <t>CUSTOMS_CURRENCY</t>
-  </si>
-  <si>
-    <t>CUSTOMS_CLEARANCE</t>
-  </si>
-  <si>
-    <t>CFS_CURRENCY</t>
-  </si>
-  <si>
-    <t>CFS_TERMINAL_CHARGES</t>
-  </si>
-  <si>
-    <t>EXP_CURRENCY</t>
-  </si>
-  <si>
-    <t>EXP_DECLARATION</t>
-  </si>
-  <si>
-    <t>EXP_LIMIT</t>
-  </si>
-  <si>
-    <t>EXP_XTRA</t>
-  </si>
-  <si>
     <t>ocean</t>
   </si>
   <si>
@@ -175,12 +91,6 @@
   </si>
   <si>
     <t>USD</t>
-  </si>
-  <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>EUR</t>
   </si>
   <si>
     <t>Mumbai</t>
@@ -434,95 +344,39 @@
       <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="12"/>
       <c r="B2" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -533,13 +387,13 @@
         <v>43465.0</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J2" s="13">
         <v>39.0</v>
@@ -553,95 +407,39 @@
       <c r="M2" s="15">
         <v>4.0</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="17">
-        <v>165.0</v>
-      </c>
-      <c r="P2" s="17">
-        <v>395.0</v>
-      </c>
-      <c r="Q2" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T2" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U2" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG2" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI2" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK2" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL2" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM2" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN2" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO2" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="16"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="16"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="17"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -652,13 +450,13 @@
         <v>43465.0</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J3" s="13">
         <v>39.0</v>
@@ -672,95 +470,39 @@
       <c r="M3" s="15">
         <v>4.0</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P3" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q3" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T3" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U3" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W3" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y3" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA3" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC3" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE3" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG3" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI3" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK3" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM3" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN3" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO3" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="16"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="16"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="17"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -771,13 +513,13 @@
         <v>43465.0</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J4" s="13">
         <v>39.0</v>
@@ -791,95 +533,39 @@
       <c r="M4" s="15">
         <v>4.0</v>
       </c>
-      <c r="N4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P4" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q4" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T4" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U4" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y4" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA4" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC4" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE4" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG4" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI4" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK4" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL4" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM4" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN4" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO4" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="21"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="17"/>
     </row>
     <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="12"/>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -890,13 +576,13 @@
         <v>43465.0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J5" s="13">
         <v>39.0</v>
@@ -910,95 +596,39 @@
       <c r="M5" s="15">
         <v>4.0</v>
       </c>
-      <c r="N5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P5" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T5" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U5" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W5" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y5" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA5" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC5" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE5" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG5" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI5" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK5" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL5" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM5" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN5" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO5" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N5" s="16"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="19"/>
+      <c r="AO5" s="17"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -1009,13 +639,13 @@
         <v>43465.0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J6" s="13">
         <v>39.0</v>
@@ -1029,95 +659,39 @@
       <c r="M6" s="15">
         <v>4.0</v>
       </c>
-      <c r="N6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P6" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T6" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U6" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W6" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y6" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA6" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC6" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE6" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG6" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI6" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK6" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM6" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN6" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO6" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="19"/>
+      <c r="AO6" s="17"/>
     </row>
     <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -1128,13 +702,13 @@
         <v>43465.0</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J7" s="13">
         <v>39.0</v>
@@ -1148,95 +722,39 @@
       <c r="M7" s="15">
         <v>4.0</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P7" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T7" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U7" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W7" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA7" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC7" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG7" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI7" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK7" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL7" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM7" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN7" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO7" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="16"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="16"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="18"/>
+      <c r="AN7" s="19"/>
+      <c r="AO7" s="17"/>
     </row>
     <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -1247,13 +765,13 @@
         <v>43465.0</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J8" s="13">
         <v>39.0</v>
@@ -1267,95 +785,39 @@
       <c r="M8" s="15">
         <v>4.0</v>
       </c>
-      <c r="N8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P8" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q8" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T8" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U8" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W8" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA8" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC8" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE8" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG8" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI8" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK8" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL8" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM8" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN8" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO8" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N8" s="16"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="21"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="19"/>
+      <c r="AO8" s="17"/>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1366,13 +828,13 @@
         <v>43465.0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J9" s="13">
         <v>39.0</v>
@@ -1386,95 +848,39 @@
       <c r="M9" s="15">
         <v>4.0</v>
       </c>
-      <c r="N9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P9" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S9" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T9" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U9" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W9" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y9" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA9" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC9" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE9" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG9" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI9" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK9" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL9" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM9" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN9" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO9" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N9" s="16"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="16"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="16"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="21"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="19"/>
+      <c r="AO9" s="17"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -1485,13 +891,13 @@
         <v>43465.0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J10" s="13">
         <v>39.0</v>
@@ -1505,95 +911,39 @@
       <c r="M10" s="15">
         <v>4.0</v>
       </c>
-      <c r="N10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O10" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P10" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q10" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S10" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T10" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U10" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W10" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y10" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA10" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC10" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE10" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG10" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI10" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK10" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL10" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM10" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN10" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO10" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N10" s="16"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="16"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="16"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="16"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="16"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="16"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="16"/>
+      <c r="AM10" s="18"/>
+      <c r="AN10" s="19"/>
+      <c r="AO10" s="17"/>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1604,16 +954,16 @@
         <v>43465.0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J11" s="13">
-        <v>16.0</v>
+        <v>39.0</v>
       </c>
       <c r="K11" s="13">
         <v>1.25</v>
@@ -1624,95 +974,39 @@
       <c r="M11" s="15">
         <v>4.0</v>
       </c>
-      <c r="N11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O11" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P11" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q11" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S11" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T11" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U11" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V11" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W11" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y11" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA11" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC11" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE11" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG11" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI11" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK11" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM11" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN11" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO11" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N11" s="16"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="16"/>
+      <c r="AI11" s="18"/>
+      <c r="AJ11" s="16"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="16"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="19"/>
+      <c r="AO11" s="17"/>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1723,16 +1017,16 @@
         <v>43465.0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J12" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K12" s="13">
         <v>1.5</v>
@@ -1743,95 +1037,39 @@
       <c r="M12" s="15">
         <v>4.0</v>
       </c>
-      <c r="N12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O12" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P12" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q12" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S12" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T12" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U12" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W12" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y12" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA12" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC12" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE12" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG12" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI12" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ12" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK12" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL12" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM12" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN12" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO12" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="16"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="16"/>
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="16"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="16"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="16"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="21"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="19"/>
+      <c r="AO12" s="17"/>
     </row>
     <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1842,16 +1080,16 @@
         <v>43465.0</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J13" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K13" s="13">
         <v>1.5</v>
@@ -1862,95 +1100,39 @@
       <c r="M13" s="15">
         <v>4.0</v>
       </c>
-      <c r="N13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O13" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P13" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q13" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S13" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T13" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U13" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W13" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y13" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA13" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC13" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE13" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG13" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI13" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ13" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK13" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL13" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM13" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN13" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO13" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N13" s="16"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="16"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="18"/>
+      <c r="AL13" s="21"/>
+      <c r="AM13" s="18"/>
+      <c r="AN13" s="19"/>
+      <c r="AO13" s="17"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1961,16 +1143,16 @@
         <v>43465.0</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J14" s="26">
-        <v>20.0</v>
+      <c r="J14" s="13">
+        <v>39.0</v>
       </c>
       <c r="K14" s="26">
         <v>1.5</v>
@@ -1981,95 +1163,39 @@
       <c r="M14" s="26">
         <v>4.0</v>
       </c>
-      <c r="N14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O14" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P14" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q14" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S14" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T14" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U14" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V14" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W14" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y14" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA14" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC14" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE14" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG14" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI14" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK14" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL14" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM14" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN14" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO14" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N14" s="16"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="16"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="16"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="16"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="16"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="16"/>
+      <c r="AM14" s="18"/>
+      <c r="AN14" s="19"/>
+      <c r="AO14" s="17"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2080,16 +1206,16 @@
         <v>43465.0</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J15" s="26">
-        <v>20.0</v>
+      <c r="J15" s="13">
+        <v>39.0</v>
       </c>
       <c r="K15" s="26">
         <v>1.5</v>
@@ -2100,95 +1226,39 @@
       <c r="M15" s="26">
         <v>4.0</v>
       </c>
-      <c r="N15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O15" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P15" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q15" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S15" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T15" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U15" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W15" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y15" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA15" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC15" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE15" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG15" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI15" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK15" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM15" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN15" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO15" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N15" s="16"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="16"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="16"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="16"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="16"/>
+      <c r="AM15" s="18"/>
+      <c r="AN15" s="19"/>
+      <c r="AO15" s="17"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2199,16 +1269,16 @@
         <v>43465.0</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J16" s="26">
-        <v>20.0</v>
+      <c r="J16" s="13">
+        <v>39.0</v>
       </c>
       <c r="K16" s="26">
         <v>1.5</v>
@@ -2219,95 +1289,39 @@
       <c r="M16" s="26">
         <v>4.0</v>
       </c>
-      <c r="N16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O16" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P16" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q16" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S16" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T16" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U16" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V16" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W16" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y16" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA16" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC16" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE16" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG16" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI16" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK16" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM16" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN16" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO16" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="18"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="16"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="18"/>
+      <c r="AL16" s="16"/>
+      <c r="AM16" s="18"/>
+      <c r="AN16" s="19"/>
+      <c r="AO16" s="17"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" s="13" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2318,16 +1332,16 @@
         <v>43465.0</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J17" s="26">
-        <v>20.0</v>
+      <c r="J17" s="13">
+        <v>39.0</v>
       </c>
       <c r="K17" s="26">
         <v>1.5</v>
@@ -2338,95 +1352,39 @@
       <c r="M17" s="26">
         <v>4.0</v>
       </c>
-      <c r="N17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P17" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q17" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S17" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T17" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U17" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W17" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y17" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA17" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC17" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE17" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG17" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI17" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK17" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM17" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN17" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO17" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N17" s="16"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="16"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="16"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="19"/>
+      <c r="AO17" s="17"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="12"/>
       <c r="B18" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -2437,16 +1395,16 @@
         <v>43465.0</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J18" s="15">
-        <v>15.0</v>
+      <c r="J18" s="13">
+        <v>39.0</v>
       </c>
       <c r="K18" s="13">
         <v>1.0</v>
@@ -2457,95 +1415,39 @@
       <c r="M18" s="15">
         <v>4.0</v>
       </c>
-      <c r="N18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" s="17">
-        <v>165.0</v>
-      </c>
-      <c r="P18" s="17">
-        <v>395.0</v>
-      </c>
-      <c r="Q18" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S18" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T18" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U18" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V18" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W18" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y18" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA18" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB18" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC18" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE18" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG18" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI18" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK18" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM18" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN18" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO18" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N18" s="16"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="18"/>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="18"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="18"/>
+      <c r="AF18" s="16"/>
+      <c r="AG18" s="18"/>
+      <c r="AH18" s="16"/>
+      <c r="AI18" s="18"/>
+      <c r="AJ18" s="16"/>
+      <c r="AK18" s="18"/>
+      <c r="AL18" s="16"/>
+      <c r="AM18" s="18"/>
+      <c r="AN18" s="19"/>
+      <c r="AO18" s="17"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2556,16 +1458,16 @@
         <v>43465.0</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J19" s="15">
-        <v>15.0</v>
+      <c r="J19" s="13">
+        <v>39.0</v>
       </c>
       <c r="K19" s="13">
         <v>1.0</v>
@@ -2576,95 +1478,39 @@
       <c r="M19" s="15">
         <v>4.0</v>
       </c>
-      <c r="N19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O19" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P19" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q19" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S19" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T19" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U19" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W19" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y19" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA19" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC19" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE19" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG19" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI19" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK19" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM19" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN19" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO19" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="16"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="18"/>
+      <c r="AF19" s="16"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="18"/>
+      <c r="AJ19" s="16"/>
+      <c r="AK19" s="18"/>
+      <c r="AL19" s="16"/>
+      <c r="AM19" s="18"/>
+      <c r="AN19" s="19"/>
+      <c r="AO19" s="17"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2675,16 +1521,16 @@
         <v>43465.0</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J20" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K20" s="13">
         <v>1.5</v>
@@ -2695,95 +1541,39 @@
       <c r="M20" s="15">
         <v>4.0</v>
       </c>
-      <c r="N20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O20" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P20" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q20" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S20" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T20" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U20" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W20" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y20" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA20" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC20" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE20" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG20" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI20" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK20" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL20" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM20" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN20" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO20" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N20" s="16"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="18"/>
+      <c r="AB20" s="16"/>
+      <c r="AC20" s="18"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="18"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="18"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="18"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="18"/>
+      <c r="AL20" s="21"/>
+      <c r="AM20" s="18"/>
+      <c r="AN20" s="19"/>
+      <c r="AO20" s="17"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2794,16 +1584,16 @@
         <v>43465.0</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J21" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K21" s="13">
         <v>1.5</v>
@@ -2814,95 +1604,39 @@
       <c r="M21" s="15">
         <v>4.0</v>
       </c>
-      <c r="N21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O21" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P21" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q21" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S21" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T21" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U21" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W21" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y21" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA21" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC21" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE21" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG21" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI21" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK21" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL21" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM21" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN21" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO21" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N21" s="16"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="16"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="16"/>
+      <c r="AG21" s="18"/>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="18"/>
+      <c r="AJ21" s="16"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="21"/>
+      <c r="AM21" s="18"/>
+      <c r="AN21" s="19"/>
+      <c r="AO21" s="17"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2913,16 +1647,16 @@
         <v>43465.0</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J22" s="13">
-        <v>25.0</v>
+        <v>39.0</v>
       </c>
       <c r="K22" s="13">
         <v>2.0</v>
@@ -2933,95 +1667,39 @@
       <c r="M22" s="15">
         <v>4.0</v>
       </c>
-      <c r="N22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P22" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q22" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S22" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T22" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U22" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V22" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W22" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y22" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA22" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC22" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE22" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG22" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI22" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK22" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM22" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN22" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO22" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="18"/>
+      <c r="AB22" s="16"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="18"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="18"/>
+      <c r="AH22" s="16"/>
+      <c r="AI22" s="18"/>
+      <c r="AJ22" s="16"/>
+      <c r="AK22" s="18"/>
+      <c r="AL22" s="21"/>
+      <c r="AM22" s="18"/>
+      <c r="AN22" s="19"/>
+      <c r="AO22" s="17"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -3032,16 +1710,16 @@
         <v>43465.0</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J23" s="13">
-        <v>25.0</v>
+        <v>39.0</v>
       </c>
       <c r="K23" s="13">
         <v>2.0</v>
@@ -3052,95 +1730,39 @@
       <c r="M23" s="15">
         <v>4.0</v>
       </c>
-      <c r="N23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O23" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P23" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q23" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S23" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T23" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U23" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W23" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y23" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA23" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC23" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE23" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG23" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI23" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK23" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL23" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM23" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN23" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO23" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="18"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="16"/>
+      <c r="AG23" s="18"/>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="18"/>
+      <c r="AJ23" s="16"/>
+      <c r="AK23" s="18"/>
+      <c r="AL23" s="21"/>
+      <c r="AM23" s="18"/>
+      <c r="AN23" s="19"/>
+      <c r="AO23" s="17"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -3151,16 +1773,16 @@
         <v>43465.0</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J24" s="13">
-        <v>12.0</v>
+        <v>39.0</v>
       </c>
       <c r="K24" s="13">
         <v>1.0</v>
@@ -3171,95 +1793,39 @@
       <c r="M24" s="15">
         <v>4.0</v>
       </c>
-      <c r="N24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O24" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P24" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q24" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S24" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T24" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U24" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V24" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W24" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y24" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA24" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC24" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE24" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG24" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI24" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK24" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL24" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM24" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN24" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO24" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="18"/>
+      <c r="AB24" s="16"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="16"/>
+      <c r="AG24" s="18"/>
+      <c r="AH24" s="16"/>
+      <c r="AI24" s="18"/>
+      <c r="AJ24" s="16"/>
+      <c r="AK24" s="18"/>
+      <c r="AL24" s="21"/>
+      <c r="AM24" s="18"/>
+      <c r="AN24" s="19"/>
+      <c r="AO24" s="17"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -3270,16 +1836,16 @@
         <v>43465.0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J25" s="13">
-        <v>12.0</v>
+        <v>39.0</v>
       </c>
       <c r="K25" s="13">
         <v>1.0</v>
@@ -3290,95 +1856,39 @@
       <c r="M25" s="15">
         <v>4.0</v>
       </c>
-      <c r="N25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O25" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P25" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q25" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S25" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T25" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U25" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V25" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W25" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y25" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA25" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC25" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE25" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG25" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI25" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK25" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL25" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM25" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN25" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO25" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N25" s="16"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="16"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="16"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="16"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="16"/>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="21"/>
+      <c r="AM25" s="18"/>
+      <c r="AN25" s="19"/>
+      <c r="AO25" s="17"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -3389,16 +1899,16 @@
         <v>43465.0</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J26" s="13">
-        <v>16.0</v>
+        <v>39.0</v>
       </c>
       <c r="K26" s="13">
         <v>1.25</v>
@@ -3409,95 +1919,39 @@
       <c r="M26" s="15">
         <v>4.0</v>
       </c>
-      <c r="N26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="O26" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P26" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q26" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S26" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T26" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U26" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V26" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W26" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y26" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA26" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB26" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC26" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE26" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG26" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI26" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK26" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AM26" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN26" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO26" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N26" s="16"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="16"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="16"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="16"/>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="16"/>
+      <c r="AM26" s="18"/>
+      <c r="AN26" s="19"/>
+      <c r="AO26" s="17"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -3508,16 +1962,16 @@
         <v>43465.0</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J27" s="13">
-        <v>16.0</v>
+        <v>39.0</v>
       </c>
       <c r="K27" s="13">
         <v>1.25</v>
@@ -3528,95 +1982,39 @@
       <c r="M27" s="15">
         <v>4.0</v>
       </c>
-      <c r="N27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O27" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P27" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q27" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S27" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T27" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U27" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V27" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W27" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y27" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA27" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC27" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE27" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG27" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI27" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK27" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL27" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM27" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN27" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO27" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="18"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="16"/>
+      <c r="AE27" s="18"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="16"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="16"/>
+      <c r="AM27" s="18"/>
+      <c r="AN27" s="19"/>
+      <c r="AO27" s="17"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -3627,16 +2025,16 @@
         <v>43465.0</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J28" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K28" s="13">
         <v>1.5</v>
@@ -3647,95 +2045,39 @@
       <c r="M28" s="15">
         <v>4.0</v>
       </c>
-      <c r="N28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O28" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P28" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q28" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S28" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T28" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U28" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W28" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y28" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA28" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC28" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE28" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG28" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI28" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK28" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL28" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM28" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN28" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO28" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N28" s="16"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="16"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="16"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="16"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="21"/>
+      <c r="AM28" s="18"/>
+      <c r="AN28" s="19"/>
+      <c r="AO28" s="17"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -3746,16 +2088,16 @@
         <v>43465.0</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J29" s="13">
-        <v>20.0</v>
+        <v>39.0</v>
       </c>
       <c r="K29" s="13">
         <v>1.5</v>
@@ -3766,95 +2108,39 @@
       <c r="M29" s="15">
         <v>4.0</v>
       </c>
-      <c r="N29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="O29" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P29" s="20">
-        <v>395.0</v>
-      </c>
-      <c r="Q29" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="S29" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T29" s="20">
-        <v>50.0</v>
-      </c>
-      <c r="U29" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W29" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y29" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA29" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC29" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE29" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG29" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI29" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ29" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK29" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL29" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM29" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN29" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO29" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N29" s="16"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="16"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="16"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="16"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="16"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="16"/>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="21"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="19"/>
+      <c r="AO29" s="17"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -3865,16 +2151,16 @@
         <v>43465.0</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J30" s="26">
-        <v>20.0</v>
+      <c r="J30" s="13">
+        <v>39.0</v>
       </c>
       <c r="K30" s="26">
         <v>1.5</v>
@@ -3885,95 +2171,39 @@
       <c r="M30" s="26">
         <v>4.0</v>
       </c>
-      <c r="N30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O30" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P30" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q30" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S30" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T30" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U30" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V30" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W30" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y30" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA30" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC30" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE30" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG30" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI30" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK30" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL30" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM30" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN30" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO30" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N30" s="16"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="18"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="18"/>
+      <c r="AB30" s="16"/>
+      <c r="AC30" s="18"/>
+      <c r="AD30" s="16"/>
+      <c r="AE30" s="18"/>
+      <c r="AF30" s="16"/>
+      <c r="AG30" s="18"/>
+      <c r="AH30" s="16"/>
+      <c r="AI30" s="18"/>
+      <c r="AJ30" s="16"/>
+      <c r="AK30" s="18"/>
+      <c r="AL30" s="16"/>
+      <c r="AM30" s="18"/>
+      <c r="AN30" s="19"/>
+      <c r="AO30" s="17"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -3984,16 +2214,16 @@
         <v>43465.0</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J31" s="26">
-        <v>20.0</v>
+      <c r="J31" s="13">
+        <v>39.0</v>
       </c>
       <c r="K31" s="26">
         <v>1.5</v>
@@ -4004,95 +2234,39 @@
       <c r="M31" s="26">
         <v>4.0</v>
       </c>
-      <c r="N31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O31" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P31" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q31" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S31" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T31" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U31" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V31" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W31" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y31" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA31" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC31" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE31" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG31" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI31" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK31" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL31" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM31" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN31" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO31" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N31" s="16"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="18"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="18"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="18"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="18"/>
+      <c r="AB31" s="16"/>
+      <c r="AC31" s="18"/>
+      <c r="AD31" s="16"/>
+      <c r="AE31" s="18"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="18"/>
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="18"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="18"/>
+      <c r="AL31" s="16"/>
+      <c r="AM31" s="18"/>
+      <c r="AN31" s="19"/>
+      <c r="AO31" s="17"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -4103,16 +2277,16 @@
         <v>43465.0</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J32" s="26">
-        <v>20.0</v>
+      <c r="J32" s="13">
+        <v>39.0</v>
       </c>
       <c r="K32" s="26">
         <v>1.5</v>
@@ -4123,95 +2297,39 @@
       <c r="M32" s="26">
         <v>4.0</v>
       </c>
-      <c r="N32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O32" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P32" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q32" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S32" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T32" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U32" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V32" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W32" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y32" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA32" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC32" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE32" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG32" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI32" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK32" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL32" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM32" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN32" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO32" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N32" s="16"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="16"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="16"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="16"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="16"/>
+      <c r="AG32" s="18"/>
+      <c r="AH32" s="16"/>
+      <c r="AI32" s="18"/>
+      <c r="AJ32" s="16"/>
+      <c r="AK32" s="18"/>
+      <c r="AL32" s="16"/>
+      <c r="AM32" s="18"/>
+      <c r="AN32" s="19"/>
+      <c r="AO32" s="17"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" s="13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -4222,16 +2340,16 @@
         <v>43465.0</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
-      <c r="J33" s="26">
-        <v>20.0</v>
+      <c r="J33" s="13">
+        <v>39.0</v>
       </c>
       <c r="K33" s="26">
         <v>1.5</v>
@@ -4242,90 +2360,34 @@
       <c r="M33" s="26">
         <v>4.0</v>
       </c>
-      <c r="N33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O33" s="18">
-        <v>165.0</v>
-      </c>
-      <c r="P33" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="Q33" s="18">
-        <v>395.0</v>
-      </c>
-      <c r="R33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="S33" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="T33" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="U33" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="V33" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="W33" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="X33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y33" s="18">
-        <v>625.0</v>
-      </c>
-      <c r="Z33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA33" s="18">
-        <v>675.0</v>
-      </c>
-      <c r="AB33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC33" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AD33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE33" s="18">
-        <v>5.0</v>
-      </c>
-      <c r="AF33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG33" s="18">
-        <v>50.0</v>
-      </c>
-      <c r="AH33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI33" s="18">
-        <v>25.0</v>
-      </c>
-      <c r="AJ33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK33" s="18">
-        <v>22.0</v>
-      </c>
-      <c r="AL33" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM33" s="18">
-        <v>400.0</v>
-      </c>
-      <c r="AN33" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="AO33" s="17">
-        <v>50.0</v>
-      </c>
+      <c r="N33" s="16"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="18"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="18"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="18"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="18"/>
+      <c r="AB33" s="16"/>
+      <c r="AC33" s="18"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="18"/>
+      <c r="AF33" s="16"/>
+      <c r="AG33" s="18"/>
+      <c r="AH33" s="16"/>
+      <c r="AI33" s="18"/>
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="18"/>
+      <c r="AL33" s="16"/>
+      <c r="AM33" s="18"/>
+      <c r="AN33" s="19"/>
+      <c r="AO33" s="17"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="12"/>

</xml_diff>